<commit_message>
CCSB Combined Outflow, 11452901, 4_wy2016-18, pTHg,  fTHg, wwTHg: Updated model results; new folder for rloadest Combined Outflow; new folder for Sigma Plot Combined Outflow in 4_wy2016-18; Updated Loads Progress sheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/4_wy2016-2018/4_pTHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/4_wy2016-2018/4_pTHg Model Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\4_wy2016-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2105A1DF-2931-4177-B1E0-E506E8B80385}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088FDC8C-CF6D-4DE6-A101-3CBC27835050}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pTHg wy2016-18 Model Results" sheetId="2" r:id="rId1"/>
-    <sheet name="Outlet_30ct" sheetId="9" r:id="rId2"/>
-    <sheet name="Rumsey" sheetId="8" r:id="rId3"/>
+    <sheet name="Combined" sheetId="10" r:id="rId2"/>
+    <sheet name="Outlet_30ct" sheetId="9" r:id="rId3"/>
+    <sheet name="Rumsey" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="669">
   <si>
     <t>Model #</t>
   </si>
@@ -1489,6 +1490,594 @@
   </si>
   <si>
     <t>26.7, 32.0, 61.4</t>
+  </si>
+  <si>
+    <t>Combined Outflow pTHg</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm1 &lt;- loadReg(pTHg ~model(1), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(1), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 36</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0238</t>
+  </si>
+  <si>
+    <t>(Intercept)   -2.346     0.1634  -14.36       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.507     0.0967   15.59       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9522</t>
+  </si>
+  <si>
+    <t>R-squared: 87.72 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 75.5 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2402</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4948</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.58 1.69 4.93 6.23 6.43</t>
+  </si>
+  <si>
+    <t>Obs   0 0.02 0.16 1.39 4.82 5.42 8.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.6 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.869</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm2 &lt;- loadReg(pTHg ~model(2), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(2), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm2</t>
+  </si>
+  <si>
+    <t>(Intercept) -2.44464    0.26221 -9.3232  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.50706    0.09781 15.4088  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.03444    0.07127  0.4833  0.6143</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9742</t>
+  </si>
+  <si>
+    <t>R-squared: 87.81 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 75.76 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1697</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5174</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.54 1.70 5.35 6.86 7.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 18.11 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8475</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm3 &lt;- loadReg(pTHg ~model(3), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(3), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept)  -2.4259    0.16536 -14.671  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.5285    0.09479  16.125  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.4753    0.27459  -1.731  0.0769</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8994</t>
+  </si>
+  <si>
+    <t>R-squared: 88.74 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 78.63 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7418</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4281</t>
+  </si>
+  <si>
+    <t>lnQ     1.017</t>
+  </si>
+  <si>
+    <t>DECTIME 1.017</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.55 1.73 4.26 5.31 5.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.758 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8676</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm4 &lt;- loadReg(pTHg ~model(4), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(4), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.7045     0.9728 -3.8081  0.0002</t>
+  </si>
+  <si>
+    <t>lnQ           1.4257     0.1030 13.8453  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.7678     0.8526  0.9006  0.3425</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   1.4959     0.8228  1.8180  0.0600</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8727</t>
+  </si>
+  <si>
+    <t>R-squared: 89.41 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 80.83 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0619</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3736</t>
+  </si>
+  <si>
+    <t>lnQ         1.237</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.973</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 4.201</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.41 1.80 5.20 5.86 6.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 13.22 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8587</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm5 &lt;- loadReg(pTHg ~model(5), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(5), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm5</t>
+  </si>
+  <si>
+    <t>(Intercept) -2.67640    0.27610  -9.693  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.53332    0.09449  16.227  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.08148    0.07209   1.130  0.2352</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.58129    0.28909  -2.011  0.0385</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.892</t>
+  </si>
+  <si>
+    <t>R-squared: 89.18 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 80.04 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.5327</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.455</t>
+  </si>
+  <si>
+    <t>lnQ     1.019</t>
+  </si>
+  <si>
+    <t>lnQ2    1.118</t>
+  </si>
+  <si>
+    <t>DECTIME 1.137</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.44 1.71 5.02 6.59 7.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 13.97 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8594</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm6 &lt;- loadReg(pTHg ~model(6), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(6), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Estimate Std. Error  z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) -3.676892    1.03155 -3.56444  0.0004</t>
+  </si>
+  <si>
+    <t>lnQ          1.425604    0.10461 13.62718  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.006995    0.07504 -0.09321  0.9200</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.751998    0.88261  0.85202  0.3613</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  1.498342    0.83629  1.79165  0.0596</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9006</t>
+  </si>
+  <si>
+    <t>G-squared: 80.84 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0582</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3685</t>
+  </si>
+  <si>
+    <t>lnQ         1.238</t>
+  </si>
+  <si>
+    <t>lnQ2        1.199</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.126</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 4.205</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.42 1.82 5.06 5.55 6.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.88 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8645</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm7 &lt;- loadReg(pTHg ~model(7), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(7), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.1638     1.0698 -2.9574  0.0028</t>
+  </si>
+  <si>
+    <t>lnQ           1.4698     0.1089 13.4910  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.3600     0.3048 -1.1810  0.2082</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.2626     0.9492  0.2767  0.7657</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   0.9889     0.9236  1.0707  0.2529</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8621</t>
+  </si>
+  <si>
+    <t>R-squared: 89.87 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.41 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2268</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3697</t>
+  </si>
+  <si>
+    <t>lnQ         1.402</t>
+  </si>
+  <si>
+    <t>DECTIME     1.308</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.985</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.359</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.44 1.68 4.47 5.59 6.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 6.848 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8918</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm8 &lt;- loadReg(pTHg ~model(8), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(8), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm8</t>
+  </si>
+  <si>
+    <t>(Intercept) -3.21136    1.09266 -2.9390  0.0025</t>
+  </si>
+  <si>
+    <t>lnQ          1.47595    0.11174 13.2088  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.02962    0.08031  0.3688  0.6865</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.40603    0.33342 -1.2178  0.1875</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.26510    0.96276  0.2754  0.7631</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.91368    0.95872  0.9530  0.3001</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8868</t>
+  </si>
+  <si>
+    <t>R-squared: 89.91 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.57 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2025</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3885</t>
+  </si>
+  <si>
+    <t>lnQ         1.434</t>
+  </si>
+  <si>
+    <t>lnQ2        1.395</t>
+  </si>
+  <si>
+    <t>DECTIME     1.521</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.986</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.613</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.43 1.69 4.74 5.92 6.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 10.71 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8889</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm9 &lt;- loadReg(pTHg ~model(9), data = pTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(9), data = pTHg_Combined, flow = "Flow",  :</t>
+  </si>
+  <si>
+    <t>&gt; pTHg_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept) -2.51841    1.13491 -2.2190  0.0175</t>
+  </si>
+  <si>
+    <t>lnQ          1.64694    0.14768 11.1521  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.02989    0.07787  0.3838  0.6693</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.58864    0.34062 -1.7282  0.0603</t>
+  </si>
+  <si>
+    <t>DECTIME2     0.92441    0.54249  1.7040  0.0638</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.89689    1.15612 -0.7758  0.3898</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.24044    1.01015  0.2380  0.7910</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8339</t>
+  </si>
+  <si>
+    <t>R-squared: 90.83 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 86.01 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3927</t>
+  </si>
+  <si>
+    <t>lnQ         2.664</t>
+  </si>
+  <si>
+    <t>DECTIME2    2.439</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 7.646</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 6.627</t>
+  </si>
+  <si>
+    <t>Est   0 0.02 0.34 1.75 4.30 7.43 8.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.15 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8776</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 36; Period of record: 2016-01-20 to 2018-04-08</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(1), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(2), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(3), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(4), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(5), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(6), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(7), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(8), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(pTHg ~ model(9), data = pTHg_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>20.97, 26.22, 29.88</t>
+  </si>
+  <si>
+    <t>26.42, 26.83, 61.40</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +2323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1867,6 +2456,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1891,14 +2486,134 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2431,11 +3146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE30"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P18" sqref="P18"/>
+      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,24 +3172,24 @@
       <c r="A1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="50"/>
+      <c r="M1" s="52"/>
       <c r="O1" s="21"/>
       <c r="R1" s="21"/>
     </row>
@@ -2611,18 +3326,18 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="48"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="57"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="59"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="O6" s="48"/>
@@ -2632,22 +3347,22 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="48"/>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="54" t="s">
         <v>309</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="51" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="51"/>
+      <c r="M7" s="53"/>
       <c r="O7" s="48"/>
       <c r="P7" s="48"/>
       <c r="R7" s="48"/>
@@ -2839,7 +3554,7 @@
       <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="51">
         <v>0.13739999999999999</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -3245,40 +3960,46 @@
       <c r="P18" s="48"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B19" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="R19" s="1"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="57" t="s">
+        <v>473</v>
+      </c>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="R19" s="50"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
-        <v>271</v>
-      </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="51" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="54" t="s">
+        <v>657</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="51"/>
-      <c r="R20" s="1"/>
+      <c r="M20" s="53"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="R20" s="50"/>
     </row>
     <row r="21" spans="1:31" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -3362,45 +4083,49 @@
         <v>7</v>
       </c>
       <c r="I22" s="6">
-        <v>91.51</v>
+        <v>87.72</v>
       </c>
       <c r="J22" s="6">
-        <v>0.40329999999999999</v>
+        <v>0.2402</v>
       </c>
       <c r="K22" s="6">
-        <v>0.44669999999999999</v>
+        <v>0.49480000000000002</v>
       </c>
       <c r="L22" s="6">
-        <v>50.38</v>
+        <v>11.6</v>
       </c>
       <c r="M22" s="6">
-        <v>0.45939999999999998</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="N22" s="6">
         <v>1</v>
       </c>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
+      <c r="O22" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="P22" s="31" t="s">
+        <v>667</v>
+      </c>
       <c r="Q22" s="31"/>
       <c r="R22" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD22" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="AB22" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="38">
+      <c r="A23" s="50">
         <v>2</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
       </c>
       <c r="C23" s="19">
-        <v>0.33689999999999998</v>
+        <v>0.61429999999999996</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>9</v>
@@ -3417,22 +4142,22 @@
       <c r="H23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="41">
-        <v>91.66</v>
-      </c>
-      <c r="J23" s="41">
-        <v>0.78539999999999999</v>
-      </c>
-      <c r="K23" s="41">
-        <v>0.46529999999999999</v>
-      </c>
-      <c r="L23" s="41">
-        <v>77.39</v>
-      </c>
-      <c r="M23" s="41">
-        <v>-0.21229999999999999</v>
-      </c>
-      <c r="N23" s="43">
+      <c r="I23" s="50">
+        <v>87.81</v>
+      </c>
+      <c r="J23" s="50">
+        <v>0.16969999999999999</v>
+      </c>
+      <c r="K23" s="50">
+        <v>0.51739999999999997</v>
+      </c>
+      <c r="L23" s="50">
+        <v>18.11</v>
+      </c>
+      <c r="M23" s="50">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="N23" s="50">
         <v>2</v>
       </c>
       <c r="O23" s="40"/>
@@ -3442,9 +4167,9 @@
         <v>10</v>
       </c>
       <c r="T23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD23" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="AB23" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3459,7 +4184,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="47">
-        <v>8.3999999999999995E-3</v>
+        <v>7.6899999999999996E-2</v>
       </c>
       <c r="E24" s="46" t="s">
         <v>9</v>
@@ -3470,23 +4195,23 @@
       <c r="G24" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="39" t="s">
+      <c r="H24" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I24" s="39">
-        <v>92.57</v>
+        <v>88.74</v>
       </c>
       <c r="J24" s="39">
-        <v>0.25030000000000002</v>
+        <v>0.74180000000000001</v>
       </c>
       <c r="K24" s="39">
-        <v>0.34810000000000002</v>
-      </c>
-      <c r="L24" s="31">
-        <v>25.57</v>
-      </c>
-      <c r="M24" s="31">
-        <v>0.80620000000000003</v>
+        <v>0.42809999999999998</v>
+      </c>
+      <c r="L24" s="39">
+        <v>1.758</v>
+      </c>
+      <c r="M24" s="39">
+        <v>0.86760000000000004</v>
       </c>
       <c r="N24" s="44">
         <v>3</v>
@@ -3495,23 +4220,21 @@
         <v>272</v>
       </c>
       <c r="P24" s="44" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q24" s="45" t="s">
-        <v>9</v>
-      </c>
+        <v>668</v>
+      </c>
+      <c r="Q24" s="45"/>
       <c r="R24" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD24" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="AB24" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="38">
+      <c r="A25" s="50">
         <v>4</v>
       </c>
       <c r="B25" s="6">
@@ -3527,56 +4250,56 @@
         <v>9</v>
       </c>
       <c r="F25" s="6">
-        <v>0.57930000000000004</v>
-      </c>
-      <c r="G25" s="41">
-        <v>2.4299999999999999E-2</v>
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="G25" s="50">
+        <v>0.06</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="41">
-        <v>93.45</v>
-      </c>
-      <c r="J25" s="41">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="K25" s="41">
-        <v>0.3826</v>
-      </c>
-      <c r="L25" s="41">
-        <v>60.89</v>
-      </c>
-      <c r="M25" s="41">
-        <v>8.5500000000000007E-2</v>
+      <c r="I25" s="50">
+        <v>89.41</v>
+      </c>
+      <c r="J25" s="50">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="K25" s="50">
+        <v>0.37359999999999999</v>
+      </c>
+      <c r="L25" s="50">
+        <v>13.22</v>
+      </c>
+      <c r="M25" s="50">
+        <v>0.85870000000000002</v>
       </c>
       <c r="N25" s="31">
         <v>4</v>
       </c>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
       <c r="R25" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD25" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="AB25" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="38">
+      <c r="A26" s="50">
         <v>5</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
       </c>
-      <c r="C26" s="41">
-        <v>0.1203</v>
-      </c>
-      <c r="D26" s="41">
-        <v>3.7000000000000002E-3</v>
+      <c r="C26" s="50">
+        <v>0.23519999999999999</v>
+      </c>
+      <c r="D26" s="50">
+        <v>3.85E-2</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>9</v>
@@ -3590,45 +4313,45 @@
       <c r="H26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="41">
-        <v>92.91</v>
-      </c>
-      <c r="J26" s="41">
-        <v>0.30809999999999998</v>
-      </c>
-      <c r="K26" s="41">
-        <v>0.34660000000000002</v>
-      </c>
-      <c r="L26" s="41">
-        <v>58.95</v>
-      </c>
-      <c r="M26" s="41">
-        <v>0.2283</v>
+      <c r="I26" s="50">
+        <v>89.18</v>
+      </c>
+      <c r="J26" s="50">
+        <v>0.53269999999999995</v>
+      </c>
+      <c r="K26" s="50">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="L26" s="50">
+        <v>13.97</v>
+      </c>
+      <c r="M26" s="50">
+        <v>0.85940000000000005</v>
       </c>
       <c r="N26" s="31">
         <v>5</v>
       </c>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
       <c r="R26" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD26" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="AB26" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="38">
+      <c r="A27" s="50">
         <v>6</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
       </c>
-      <c r="C27" s="41">
-        <v>0.95779999999999998</v>
+      <c r="C27" s="50">
+        <v>0.92</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>9</v>
@@ -3637,46 +4360,46 @@
         <v>9</v>
       </c>
       <c r="F27" s="6">
-        <v>0.58130000000000004</v>
-      </c>
-      <c r="G27" s="41">
-        <v>3.7199999999999997E-2</v>
+        <v>0.36130000000000001</v>
+      </c>
+      <c r="G27" s="50">
+        <v>5.96E-2</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="41">
-        <v>93.45</v>
-      </c>
-      <c r="J27" s="41">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="K27" s="41">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="L27" s="41">
-        <v>60.86</v>
-      </c>
-      <c r="M27" s="41">
-        <v>0.10199999999999999</v>
+      <c r="I27" s="50">
+        <v>89.41</v>
+      </c>
+      <c r="J27" s="50">
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="K27" s="50">
+        <v>0.36849999999999999</v>
+      </c>
+      <c r="L27" s="50">
+        <v>11.88</v>
+      </c>
+      <c r="M27" s="50">
+        <v>0.86450000000000005</v>
       </c>
       <c r="N27" s="31">
         <v>6</v>
       </c>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
       <c r="R27" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD27" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="AB27" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="38">
+      <c r="A28" s="50">
         <v>7</v>
       </c>
       <c r="B28" s="6">
@@ -3686,229 +4409,880 @@
         <v>9</v>
       </c>
       <c r="D28" s="6">
-        <v>6.25E-2</v>
+        <v>0.2082</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="6">
-        <v>0.76129999999999998</v>
-      </c>
-      <c r="G28" s="41">
-        <v>3.2899999999999999E-2</v>
+        <v>0.76570000000000005</v>
+      </c>
+      <c r="G28" s="50">
+        <v>0.25290000000000001</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="41">
-        <v>93.88</v>
-      </c>
-      <c r="J28" s="41">
-        <v>0.52610000000000001</v>
-      </c>
-      <c r="K28" s="41">
-        <v>0.32450000000000001</v>
-      </c>
-      <c r="L28" s="41">
-        <v>40.65</v>
-      </c>
-      <c r="M28" s="41">
-        <v>0.51910000000000001</v>
+      <c r="I28" s="50">
+        <v>89.87</v>
+      </c>
+      <c r="J28" s="50">
+        <v>0.2268</v>
+      </c>
+      <c r="K28" s="50">
+        <v>0.36969999999999997</v>
+      </c>
+      <c r="L28" s="50">
+        <v>6.8479999999999999</v>
+      </c>
+      <c r="M28" s="50">
+        <v>0.89180000000000004</v>
       </c>
       <c r="N28" s="31">
         <v>7</v>
       </c>
-      <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
       <c r="R28" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T28" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD28" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="AB28" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="38">
+      <c r="A29" s="50">
         <v>8</v>
       </c>
       <c r="B29" s="6">
         <v>0</v>
       </c>
-      <c r="C29" s="41">
-        <v>0.5645</v>
+      <c r="C29" s="50">
+        <v>0.6865</v>
       </c>
       <c r="D29" s="6">
-        <v>5.1299999999999998E-2</v>
+        <v>0.1875</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="6">
-        <v>0.67789999999999995</v>
+        <v>0.7631</v>
       </c>
       <c r="G29" s="6">
-        <v>8.0299999999999996E-2</v>
+        <v>0.30009999999999998</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="41">
-        <v>93.92</v>
-      </c>
-      <c r="J29" s="41">
-        <v>0.36020000000000002</v>
-      </c>
-      <c r="K29" s="41">
-        <v>0.32950000000000002</v>
-      </c>
-      <c r="L29" s="41">
-        <v>51.98</v>
-      </c>
-      <c r="M29" s="41">
-        <v>0.28899999999999998</v>
+      <c r="I29" s="50">
+        <v>89.91</v>
+      </c>
+      <c r="J29" s="50">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="K29" s="50">
+        <v>0.38850000000000001</v>
+      </c>
+      <c r="L29" s="50">
+        <v>10.71</v>
+      </c>
+      <c r="M29" s="50">
+        <v>0.88890000000000002</v>
       </c>
       <c r="N29" s="31">
         <v>8</v>
       </c>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
       <c r="R29" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T29" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD29" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="AB29" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="38">
+      <c r="A30" s="50">
         <v>9</v>
       </c>
       <c r="B30" s="6">
         <v>0</v>
       </c>
-      <c r="C30" s="41">
-        <v>4.41E-2</v>
+      <c r="C30" s="50">
+        <v>0.66930000000000001</v>
       </c>
       <c r="D30" s="6">
-        <v>0.13120000000000001</v>
+        <v>6.0299999999999999E-2</v>
       </c>
       <c r="E30" s="6">
-        <v>0</v>
+        <v>6.3799999999999996E-2</v>
       </c>
       <c r="F30" s="6">
-        <v>1.0500000000000001E-2</v>
+        <v>0.38979999999999998</v>
       </c>
       <c r="G30" s="6">
-        <v>0.45240000000000002</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="41">
-        <v>95.98</v>
-      </c>
-      <c r="J30" s="41">
-        <v>6.13E-2</v>
-      </c>
-      <c r="K30" s="41">
-        <v>9.7900000000000001E-2</v>
-      </c>
-      <c r="L30" s="41">
-        <v>51.49</v>
-      </c>
-      <c r="M30" s="41">
-        <v>-0.23599999999999999</v>
+      <c r="I30" s="50">
+        <v>90.83</v>
+      </c>
+      <c r="J30" s="50">
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="K30" s="50">
+        <v>0.39269999999999999</v>
+      </c>
+      <c r="L30" s="50">
+        <v>11.15</v>
+      </c>
+      <c r="M30" s="50">
+        <v>0.87760000000000005</v>
       </c>
       <c r="N30" s="31">
         <v>9</v>
       </c>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
       <c r="R30" s="8" t="s">
         <v>10</v>
       </c>
       <c r="T30" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB30" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B32" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B33" s="54" t="s">
+        <v>271</v>
+      </c>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="M33" s="53"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:30" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="O34" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q34" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="6">
+        <v>91.51</v>
+      </c>
+      <c r="J35" s="6">
+        <v>0.40329999999999999</v>
+      </c>
+      <c r="K35" s="6">
+        <v>0.44669999999999999</v>
+      </c>
+      <c r="L35" s="6">
+        <v>50.38</v>
+      </c>
+      <c r="M35" s="6">
+        <v>0.45939999999999998</v>
+      </c>
+      <c r="N35" s="6">
+        <v>1</v>
+      </c>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD35" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="38">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0</v>
+      </c>
+      <c r="C36" s="19">
+        <v>0.33689999999999998</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="41">
+        <v>91.66</v>
+      </c>
+      <c r="J36" s="41">
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="K36" s="41">
+        <v>0.46529999999999999</v>
+      </c>
+      <c r="L36" s="41">
+        <v>77.39</v>
+      </c>
+      <c r="M36" s="41">
+        <v>-0.21229999999999999</v>
+      </c>
+      <c r="N36" s="43">
+        <v>2</v>
+      </c>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+      <c r="Q36" s="31"/>
+      <c r="R36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD36" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="39">
+        <v>3</v>
+      </c>
+      <c r="B37" s="39">
+        <v>0</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="47">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="39">
+        <v>92.57</v>
+      </c>
+      <c r="J37" s="39">
+        <v>0.25030000000000002</v>
+      </c>
+      <c r="K37" s="39">
+        <v>0.34810000000000002</v>
+      </c>
+      <c r="L37" s="31">
+        <v>25.57</v>
+      </c>
+      <c r="M37" s="31">
+        <v>0.80620000000000003</v>
+      </c>
+      <c r="N37" s="44">
+        <v>3</v>
+      </c>
+      <c r="O37" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="P37" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q37" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD37" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="38">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.57930000000000004</v>
+      </c>
+      <c r="G38" s="41">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="41">
+        <v>93.45</v>
+      </c>
+      <c r="J38" s="41">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="K38" s="41">
+        <v>0.3826</v>
+      </c>
+      <c r="L38" s="41">
+        <v>60.89</v>
+      </c>
+      <c r="M38" s="41">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="N38" s="31">
+        <v>4</v>
+      </c>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
+      <c r="R38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD38" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="38">
+        <v>5</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0</v>
+      </c>
+      <c r="C39" s="41">
+        <v>0.1203</v>
+      </c>
+      <c r="D39" s="41">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="41">
+        <v>92.91</v>
+      </c>
+      <c r="J39" s="41">
+        <v>0.30809999999999998</v>
+      </c>
+      <c r="K39" s="41">
+        <v>0.34660000000000002</v>
+      </c>
+      <c r="L39" s="41">
+        <v>58.95</v>
+      </c>
+      <c r="M39" s="41">
+        <v>0.2283</v>
+      </c>
+      <c r="N39" s="31">
+        <v>5</v>
+      </c>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="R39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T39" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD39" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="38">
+        <v>6</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0</v>
+      </c>
+      <c r="C40" s="41">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0.58130000000000004</v>
+      </c>
+      <c r="G40" s="41">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="41">
+        <v>93.45</v>
+      </c>
+      <c r="J40" s="41">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="K40" s="41">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="L40" s="41">
+        <v>60.86</v>
+      </c>
+      <c r="M40" s="41">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="N40" s="31">
+        <v>6</v>
+      </c>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="R40" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T40" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD40" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="38">
+        <v>7</v>
+      </c>
+      <c r="B41" s="6">
+        <v>0</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="6">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="6">
+        <v>0.76129999999999998</v>
+      </c>
+      <c r="G41" s="41">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="41">
+        <v>93.88</v>
+      </c>
+      <c r="J41" s="41">
+        <v>0.52610000000000001</v>
+      </c>
+      <c r="K41" s="41">
+        <v>0.32450000000000001</v>
+      </c>
+      <c r="L41" s="41">
+        <v>40.65</v>
+      </c>
+      <c r="M41" s="41">
+        <v>0.51910000000000001</v>
+      </c>
+      <c r="N41" s="31">
+        <v>7</v>
+      </c>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="R41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD41" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="38">
+        <v>8</v>
+      </c>
+      <c r="B42" s="6">
+        <v>0</v>
+      </c>
+      <c r="C42" s="41">
+        <v>0.5645</v>
+      </c>
+      <c r="D42" s="6">
+        <v>5.1299999999999998E-2</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0.67789999999999995</v>
+      </c>
+      <c r="G42" s="6">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="41">
+        <v>93.92</v>
+      </c>
+      <c r="J42" s="41">
+        <v>0.36020000000000002</v>
+      </c>
+      <c r="K42" s="41">
+        <v>0.32950000000000002</v>
+      </c>
+      <c r="L42" s="41">
+        <v>51.98</v>
+      </c>
+      <c r="M42" s="41">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="N42" s="31">
+        <v>8</v>
+      </c>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
+      <c r="R42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T42" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD42" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="38">
+        <v>9</v>
+      </c>
+      <c r="B43" s="6">
+        <v>0</v>
+      </c>
+      <c r="C43" s="41">
+        <v>4.41E-2</v>
+      </c>
+      <c r="D43" s="6">
+        <v>0.13120000000000001</v>
+      </c>
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+      <c r="F43" s="6">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.45240000000000002</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="41">
+        <v>95.98</v>
+      </c>
+      <c r="J43" s="41">
+        <v>6.13E-2</v>
+      </c>
+      <c r="K43" s="41">
+        <v>9.7900000000000001E-2</v>
+      </c>
+      <c r="L43" s="41">
+        <v>51.49</v>
+      </c>
+      <c r="M43" s="41">
+        <v>-0.23599999999999999</v>
+      </c>
+      <c r="N43" s="31">
+        <v>9</v>
+      </c>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="R43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="T43" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AD30" s="9" t="s">
+      <c r="AD43" s="9" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="B32:K32"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="L20:M20"/>
   </mergeCells>
-  <conditionalFormatting sqref="M19 L55:L1048576">
-    <cfRule type="cellIs" dxfId="18" priority="57" operator="between">
+  <conditionalFormatting sqref="M32 L68:L1048576">
+    <cfRule type="cellIs" dxfId="30" priority="69" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="70" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="71" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19 K31:K1048576">
-    <cfRule type="cellIs" dxfId="15" priority="43" operator="lessThan">
+  <conditionalFormatting sqref="L32 K44:K1048576">
+    <cfRule type="cellIs" dxfId="27" priority="55" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="44" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="56" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35:J43">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M35:M43">
+    <cfRule type="cellIs" dxfId="24" priority="38" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="39" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="40" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L35:L43">
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="37" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36 D37 C39:C40 D39 C42:C43 D41:D43 E43 F38:G38 F40:G43">
+    <cfRule type="cellIs" dxfId="19" priority="35" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J17">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M9:M17">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:L17">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10 D11 C13:C14 D13 C16:C17 D15:D17 E17 F12:G12 F14:G17">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M19">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J30">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22:M30">
-    <cfRule type="cellIs" dxfId="12" priority="26" operator="between">
-      <formula>0.5</formula>
-      <formula>0.8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="27" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="28" operator="greaterThan">
-      <formula>0.8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L30">
-    <cfRule type="cellIs" dxfId="9" priority="24" operator="lessThan">
-      <formula>-25</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="25" operator="greaterThan">
-      <formula>25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23 D24 C26:C27 D26 C29:C30 D28:D30 E30 F25:G25 F27:G30">
-    <cfRule type="cellIs" dxfId="7" priority="23" operator="greaterThan">
-      <formula>0.1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J17">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M9:M17">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
@@ -3920,7 +5294,7 @@
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9:L17">
+  <conditionalFormatting sqref="L22:L30">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
@@ -3928,7 +5302,7 @@
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10 D11 C13:C14 D13 C16:C17 D15:D17 E17 F12:G12 F14:G17">
+  <conditionalFormatting sqref="C23 D24 C26:C27 D26 C29:C30 D28:D30 E30 F25:G25 F27:G30">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
@@ -3940,6 +5314,2475 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAA26A3-B809-4711-96F2-BAC7D8B2B0F1}">
+  <dimension ref="A1:A527"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="14" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="13"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="14" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="13"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="13"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="13"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="13"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="13"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="13"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="14" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="14" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="14" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="13"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="14" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="14" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="14" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="14" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="14" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="14" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="13"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="14" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="14" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="13"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="14" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="13"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="14" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="14" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="14" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="13"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="15" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="15" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="13"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="13"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="13"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="13"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="13"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="14" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="14" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="14" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="14" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="13"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="14" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="14" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="14" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="14" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="14" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="13"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="14" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="14" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="14" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="13"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="14" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="13"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="14" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="14" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="14" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="13"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="15" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="7" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="15" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="13"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="13"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="13"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="13"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="13"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="14" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="14" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="14" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="14" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="13"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="14" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="14" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="14" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="14" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="14" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="14" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="13"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="14" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="14" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="14" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="13"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="14" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="13"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="14" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="14" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="14" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="13"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="15" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="7" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="15" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="13"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="13"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="13"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="13"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="13"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="14" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="14" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="14" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="14" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="14" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="14" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="13"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="14" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="14" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="14" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="14" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="14" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="14" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="13"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="14" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="14" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="14" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="14" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="13"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="14" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="13"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="14" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="14" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="14" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="13"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="15" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="7" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="15" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="13"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="13"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="13"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="13"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="13"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="14" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="14" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="14" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="14" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="13"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="14" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="14" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="14" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="14" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="14" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="14" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="13"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="14" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="14" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="14" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="14" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="13"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="14" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="13"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="14" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="14" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="14" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="13"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="15" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="15" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="13"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="13"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="13"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="13"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="13"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="14" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="14" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="14" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="14" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="14" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="14" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="13"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="14" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="14" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="14" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="14" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="14" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="14" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="13"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="14" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="14" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="14" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="14" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="14" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="13"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="14" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="13"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="14" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="14" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="13"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="15" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="15" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="13"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="13"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="13"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="13"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="13"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="14" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="14" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="14" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="14" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="14" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="14" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="14" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="13"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="14" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="14" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="14" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="14" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="14" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="13"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="14" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="14" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="14" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="14" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="14" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="14" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="13"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="14" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="14" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="13"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="14" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="14" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="16"/>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="16"/>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="60" t="s">
+        <v>656</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A07B362-4B6C-4C53-91E7-80B7BF97D2BC}">
   <dimension ref="A1:A528"/>
   <sheetViews>
@@ -6409,7 +10252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7110874D-1AB5-4D4C-BDF4-3EDF5D1201E0}">
   <dimension ref="A1:A530"/>
   <sheetViews>

</xml_diff>